<commit_message>
LAU Report - Vauation
</commit_message>
<xml_diff>
--- a/app/templates/report/ltc.xlsx
+++ b/app/templates/report/ltc.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B745AC-A195-431F-83D4-B053C7E0EC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDAEA8D-B95F-4B09-A93F-465BE9D1515A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTC" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LTC!$A$3:$AF$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LTC!$A$3:$AG$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Edificio</t>
   </si>
@@ -138,10 +138,6 @@
 Pre-Capex</t>
   </si>
   <si>
-    <t>Vacant
-Value Pre-Capex</t>
-  </si>
-  <si>
     <t>Dif
 Vacant-LT</t>
   </si>
@@ -167,6 +163,16 @@
   </si>
   <si>
     <t>Código SAP</t>
+  </si>
+  <si>
+    <t>Vacant
+Value
+Pre-Capex</t>
+  </si>
+  <si>
+    <t>Residential
+Value
+Post-Capex</t>
   </si>
 </sst>
 </file>
@@ -730,46 +736,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.88671875" style="1" customWidth="1"/>
-    <col min="12" max="14" width="12.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.88671875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="15.109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" style="1" customWidth="1"/>
-    <col min="22" max="24" width="15.44140625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="22.44140625" style="1" customWidth="1"/>
-    <col min="26" max="32" width="15.44140625" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="14.44140625" style="1"/>
+    <col min="9" max="9" width="12.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" style="1" customWidth="1"/>
+    <col min="12" max="14" width="12.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="15.140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" style="1" customWidth="1"/>
+    <col min="22" max="25" width="15.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="22.42578125" style="1" customWidth="1"/>
+    <col min="27" max="33" width="15.42578125" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>40</v>
       </c>
       <c r="F1" s="18">
         <f>SUBTOTAL(9,F4:F4)</f>
@@ -803,7 +809,7 @@
       </c>
       <c r="U1" s="17"/>
       <c r="V1" s="19">
-        <f t="shared" ref="V1:AE1" si="0">SUBTOTAL(9,V4:V99999)</f>
+        <f t="shared" ref="V1:AF1" si="0">SUBTOTAL(9,V4:V99999)</f>
         <v>0</v>
       </c>
       <c r="W1" s="19">
@@ -811,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="X1" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="X1" si="1">SUBTOTAL(9,X4:X99999)</f>
         <v>0</v>
       </c>
       <c r="Y1" s="19">
@@ -842,9 +848,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF1" s="19"/>
+      <c r="AF1" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG1" s="19"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>8</v>
       </c>
@@ -878,19 +888,20 @@
       <c r="W2" s="22"/>
       <c r="X2" s="22"/>
       <c r="Y2" s="22"/>
-      <c r="Z2" s="21" t="s">
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="21"/>
       <c r="AB2" s="21"/>
-      <c r="AC2" s="22" t="s">
+      <c r="AC2" s="21"/>
+      <c r="AD2" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="AD2" s="22"/>
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
     </row>
-    <row r="3" spans="1:32" s="6" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="6" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -898,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
@@ -925,19 +936,19 @@
         <v>2</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N3" s="14" t="s">
         <v>30</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>14</v>
@@ -958,37 +969,40 @@
         <v>32</v>
       </c>
       <c r="W3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y3" s="14" t="s">
+      <c r="Z3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="AA3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AB3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AC3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AC3" s="14" t="s">
+      <c r="AD3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="AD3" s="14" t="s">
+      <c r="AE3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AE3" s="14" t="s">
+      <c r="AF3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="AG3" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1023,39 +1037,40 @@
       </c>
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
-      <c r="X4" s="10">
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10">
         <f>W4-V4</f>
         <v>0</v>
       </c>
-      <c r="Y4" s="10">
-        <f>X4-R4</f>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="10"/>
+      <c r="Z4" s="10">
+        <f>Y4-R4</f>
+        <v>0</v>
+      </c>
       <c r="AA4" s="10"/>
-      <c r="AB4" s="10">
-        <f>AA4-Z4-R4</f>
-        <v>0</v>
-      </c>
+      <c r="AB4" s="10"/>
       <c r="AC4" s="10">
-        <f>Z4+R4</f>
+        <f>AB4-AA4-R4</f>
         <v>0</v>
       </c>
       <c r="AD4" s="10">
-        <f>AA4-V4</f>
+        <f>AA4+R4</f>
         <v>0</v>
       </c>
       <c r="AE4" s="10">
-        <f>AD4-AC4</f>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="15">
-        <f>IF(AC4,AD4/AC4,0)</f>
+        <f>AB4-V4</f>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="10">
+        <f>AE4-AD4</f>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="15">
+        <f>IF(AD4,AE4/AD4,0)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AF4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:AG4" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>